<commit_message>
[SUNNY]Refactor.Data Scrapped the necessary details
</commit_message>
<xml_diff>
--- a/Flipkart Application/flipkart_iphone_uipath.xlsx
+++ b/Flipkart Application/flipkart_iphone_uipath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\UiPath\Flipkart Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20513B1E-CC47-49EF-B157-CE35BA338ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B13850-EF7D-4CD4-BCD1-54752DEA5DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3EF4C33C-18EF-49C8-835B-8FFEA671A978}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -34,6 +34,102 @@
   </si>
   <si>
     <t>rating</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Black, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>₹54,900</t>
+  </si>
+  <si>
+    <t>22,014 Ratings </t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Purple, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Black, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>₹59,900</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Red, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (White, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (White, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Red, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Green, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Green, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Yellow, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Black, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>₹69,900</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Purple, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Yellow, 128 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Green, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Red, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (White, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Purple, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 (Yellow, 256 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Midnight Green, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹79,999</t>
+  </si>
+  <si>
+    <t>5,268 Ratings </t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Silver, 512 GB)</t>
+  </si>
+  <si>
+    <t>₹1,09,999</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Space Grey, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Midnight Green, 512 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Silver, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 11 Pro (Space Grey, 512 GB)</t>
   </si>
 </sst>
 </file>
@@ -385,15 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FA2C0D-A181-498B-A64D-81FBBEAF9CAA}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,6 +503,345 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>4.5999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>